<commit_message>
test code generation module - execution data analysis for evaluation
</commit_message>
<xml_diff>
--- a/test-code-generator/configuration_analysis.xlsx
+++ b/test-code-generator/configuration_analysis.xlsx
@@ -500,7 +500,7 @@
         <v>0.07428420310449788</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2200163352833404</v>
+        <v>0.2321131094768888</v>
       </c>
       <c r="G2" t="n">
         <v>0.9111813439813872</v>
@@ -531,7 +531,7 @@
         <v>0.0753538535441081</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2102139731320689</v>
+        <v>0.2211114090295048</v>
       </c>
       <c r="G3" t="n">
         <v>0.7791074511605334</v>
@@ -562,7 +562,7 @@
         <v>0.09371188840539432</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2640845148489273</v>
+        <v>0.2545908439628514</v>
       </c>
       <c r="G4" t="n">
         <v>0.5017179725538308</v>
@@ -593,7 +593,7 @@
         <v>0.08727842956031195</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2736099442542581</v>
+        <v>0.292359944254258</v>
       </c>
       <c r="G5" t="n">
         <v>0.7108625339169765</v>
@@ -649,7 +649,7 @@
         <v>0.08499342311134304</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2558332557756678</v>
+        <v>0.2478714723361773</v>
       </c>
       <c r="G7" t="n">
         <v>0.7922215881731494</v>
@@ -680,7 +680,7 @@
         <v>0.1012206612714111</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3326221666148217</v>
+        <v>0.3421459761386313</v>
       </c>
       <c r="G8" t="n">
         <v>0.8791427387670114</v>
@@ -711,7 +711,7 @@
         <v>0.08241737011067697</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2952324621892468</v>
+        <v>0.3281994951562797</v>
       </c>
       <c r="G9" t="n">
         <v>0.8125267974608104</v>
@@ -742,7 +742,7 @@
         <v>0.0657276363698262</v>
       </c>
       <c r="F10" t="n">
-        <v>0.334253345204327</v>
+        <v>0.3233837799869357</v>
       </c>
       <c r="G10" t="n">
         <v>0.8640630327729519</v>
@@ -773,7 +773,7 @@
         <v>0.1140777195744919</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3024780101503858</v>
+        <v>0.3186070424084503</v>
       </c>
       <c r="G11" t="n">
         <v>0.8815571023392249</v>
@@ -804,7 +804,7 @@
         <v>0.08515643569758648</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3298200418124465</v>
+        <v>0.2915847476947995</v>
       </c>
       <c r="G12" t="n">
         <v>0.616442653268964</v>
@@ -835,7 +835,7 @@
         <v>0.08533426372796167</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2862226320030846</v>
+        <v>0.3097520437677905</v>
       </c>
       <c r="G13" t="n">
         <v>0.5926424133616122</v>
@@ -866,7 +866,7 @@
         <v>0.06773015082000793</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2866597135532977</v>
+        <v>0.3045168564104406</v>
       </c>
       <c r="G14" t="n">
         <v>0.799892522827738</v>
@@ -897,7 +897,7 @@
         <v>0.0704367794283077</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3246585758114504</v>
+        <v>0.2797147555867313</v>
       </c>
       <c r="G15" t="n">
         <v>0.893653131701414</v>
@@ -928,7 +928,7 @@
         <v>0.06420324406224556</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3024006053771707</v>
+        <v>0.2815672720438374</v>
       </c>
       <c r="G16" t="n">
         <v>0.7771577320072967</v>
@@ -959,7 +959,7 @@
         <v>0.107819470771444</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3099879297790363</v>
+        <v>0.3128949065232223</v>
       </c>
       <c r="G17" t="n">
         <v>0.382831176269638</v>
@@ -990,7 +990,7 @@
         <v>0.05489363236837091</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3195704746264468</v>
+        <v>0.2843140643700365</v>
       </c>
       <c r="G18" t="n">
         <v>0.6989282594950832</v>
@@ -1021,7 +1021,7 @@
         <v>0.09147199743600787</v>
       </c>
       <c r="F19" t="n">
-        <v>0.3030361939491051</v>
+        <v>0.3125600034729146</v>
       </c>
       <c r="G19" t="n">
         <v>0.7791800906011492</v>
@@ -1600,7 +1600,7 @@
         <v>0.06010144320982051</v>
       </c>
       <c r="F2" t="n">
-        <v>0.180339890082836</v>
+        <v>0.1811463416957392</v>
       </c>
       <c r="G2" t="n">
         <v>0.6465310685918169</v>
@@ -1631,7 +1631,7 @@
         <v>0.03821712062510718</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1684768357109067</v>
+        <v>0.1845024767365477</v>
       </c>
       <c r="G3" t="n">
         <v>0.9064146686587096</v>
@@ -1662,7 +1662,7 @@
         <v>0.1344235686349876</v>
       </c>
       <c r="F4" t="n">
-        <v>0.291328794478211</v>
+        <v>0.2976579084022617</v>
       </c>
       <c r="G4" t="n">
         <v>0.9081081587271729</v>
@@ -1693,7 +1693,7 @@
         <v>0.1393313676699542</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2910050226805455</v>
+        <v>0.3097550226805456</v>
       </c>
       <c r="G5" t="n">
         <v>0.6903502296784195</v>
@@ -1749,7 +1749,7 @@
         <v>0.1143157599296068</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2511612924408511</v>
+        <v>0.2543460058166472</v>
       </c>
       <c r="G7" t="n">
         <v>0.633856676927821</v>
@@ -1780,7 +1780,7 @@
         <v>0.1410223668516979</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3714292355243237</v>
+        <v>0.3309530450481332</v>
       </c>
       <c r="G8" t="n">
         <v>0.8909280568780844</v>
@@ -1836,7 +1836,7 @@
         <v>0.092481120453292</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3074232492771953</v>
+        <v>0.3155754231902388</v>
       </c>
       <c r="G10" t="n">
         <v>0.893889843775112</v>
@@ -1867,7 +1867,7 @@
         <v>0.1434735472008356</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2794478889121597</v>
+        <v>0.2875124050411919</v>
       </c>
       <c r="G11" t="n">
         <v>0.9048641310496174</v>
@@ -1898,7 +1898,7 @@
         <v>0.09645012114223925</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2764839163270338</v>
+        <v>0.2706015633858573</v>
       </c>
       <c r="G12" t="n">
         <v>0.691370862864612</v>
@@ -1929,7 +1929,7 @@
         <v>0.08993399093494622</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2778442702443801</v>
+        <v>0.3160795643620271</v>
       </c>
       <c r="G13" t="n">
         <v>0.6850179607518823</v>
@@ -1960,7 +1960,7 @@
         <v>0.0981770772598767</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2977197053667061</v>
+        <v>0.3126006577476584</v>
       </c>
       <c r="G14" t="n">
         <v>0.8190121262613472</v>
@@ -1991,7 +1991,7 @@
         <v>0.1009873426581653</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2855196017120942</v>
+        <v>0.3108005005884987</v>
       </c>
       <c r="G15" t="n">
         <v>0.855512575144713</v>
@@ -2022,7 +2022,7 @@
         <v>0.1013602641128808</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2850087495458463</v>
+        <v>0.3147706543077511</v>
       </c>
       <c r="G16" t="n">
         <v>0.8587963305103545</v>
@@ -2053,7 +2053,7 @@
         <v>0.09578916373048774</v>
       </c>
       <c r="F17" t="n">
-        <v>0.2375640356237442</v>
+        <v>0.2637268263214186</v>
       </c>
       <c r="G17" t="n">
         <v>0.8988336871127024</v>
@@ -2084,7 +2084,7 @@
         <v>0.09378996018278257</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2557689401312068</v>
+        <v>0.2846150939773607</v>
       </c>
       <c r="G18" t="n">
         <v>0.6225818585643652</v>
@@ -2115,7 +2115,7 @@
         <v>0.1658425703011601</v>
       </c>
       <c r="F19" t="n">
-        <v>0.2742317209020447</v>
+        <v>0.2789936256639494</v>
       </c>
       <c r="G19" t="n">
         <v>0.8743277846748765</v>
@@ -2197,7 +2197,7 @@
         <v>0.06002309290620027</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1920143833573574</v>
+        <v>0.2194337381960671</v>
       </c>
       <c r="G2" t="n">
         <v>0.8327897064485852</v>
@@ -2228,7 +2228,7 @@
         <v>0.04500653599041117</v>
       </c>
       <c r="F3" t="n">
-        <v>0.184050339770828</v>
+        <v>0.1853323910528792</v>
       </c>
       <c r="G3" t="n">
         <v>0.7577366593274246</v>
@@ -2259,7 +2259,7 @@
         <v>0.1521646523552269</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3414574686293478</v>
+        <v>0.3382929116673225</v>
       </c>
       <c r="G4" t="n">
         <v>0.6362074708931229</v>
@@ -2346,7 +2346,7 @@
         <v>0.09413266105154956</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2728820942261959</v>
+        <v>0.291990374480973</v>
       </c>
       <c r="G7" t="n">
         <v>0.6086277154263944</v>
@@ -2377,7 +2377,7 @@
         <v>0.2551855286176491</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4163599528234442</v>
+        <v>0.4044551909186823</v>
       </c>
       <c r="G8" t="n">
         <v>0.9083710383433946</v>
@@ -2408,7 +2408,7 @@
         <v>0.1770994089866544</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3203060235572301</v>
+        <v>0.3312950345462412</v>
       </c>
       <c r="G9" t="n">
         <v>0.6722293099207788</v>
@@ -2439,7 +2439,7 @@
         <v>0.1401184800643443</v>
       </c>
       <c r="F10" t="n">
-        <v>0.324609703874207</v>
+        <v>0.3653705734394244</v>
       </c>
       <c r="G10" t="n">
         <v>0.8997683740126933</v>
@@ -2470,7 +2470,7 @@
         <v>0.1991022788073536</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2914596241072613</v>
+        <v>0.3156531724943581</v>
       </c>
       <c r="G11" t="n">
         <v>0.8915107757736361</v>
@@ -2501,7 +2501,7 @@
         <v>0.1235704956716785</v>
       </c>
       <c r="F12" t="n">
-        <v>0.322197701141315</v>
+        <v>0.2780800540824914</v>
       </c>
       <c r="G12" t="n">
         <v>0.657042263976606</v>
@@ -2532,7 +2532,7 @@
         <v>0.1211459598520071</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3240119028029337</v>
+        <v>0.2857766086852866</v>
       </c>
       <c r="G13" t="n">
         <v>0.6668553312442823</v>
@@ -2563,7 +2563,7 @@
         <v>0.1407571790928713</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2775661355509554</v>
+        <v>0.2894708974557173</v>
       </c>
       <c r="G14" t="n">
         <v>0.6267870708289267</v>
@@ -2594,7 +2594,7 @@
         <v>0.1285980532910151</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2891449231316325</v>
+        <v>0.2863359343675875</v>
       </c>
       <c r="G15" t="n">
         <v>0.8257477823831507</v>
@@ -2625,7 +2625,7 @@
         <v>0.1350330148043991</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2856689071942169</v>
+        <v>0.3332879548132646</v>
       </c>
       <c r="G16" t="n">
         <v>0.6404359428358747</v>
@@ -2656,7 +2656,7 @@
         <v>0.20225288428756</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3440056997290209</v>
+        <v>0.3178429090313465</v>
       </c>
       <c r="G17" t="n">
         <v>0.8891023575668759</v>
@@ -2687,7 +2687,7 @@
         <v>0.1331351526019934</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3039887925534639</v>
+        <v>0.2719375105021818</v>
       </c>
       <c r="G18" t="n">
         <v>0.5760314784493452</v>
@@ -2718,7 +2718,7 @@
         <v>0.1497660078850516</v>
       </c>
       <c r="F19" t="n">
-        <v>0.2725532076602558</v>
+        <v>0.2916008267078748</v>
       </c>
       <c r="G19" t="n">
         <v>0.8617551111896915</v>
@@ -2800,7 +2800,7 @@
         <v>0.05823614108818598</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1926763845479758</v>
+        <v>0.1999344490641048</v>
       </c>
       <c r="G2" t="n">
         <v>0.7892237459460902</v>
@@ -2831,7 +2831,7 @@
         <v>0.0282416407933045</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1616512842689058</v>
+        <v>0.1680615406791622</v>
       </c>
       <c r="G3" t="n">
         <v>0.9635762266826113</v>
@@ -2862,7 +2862,7 @@
         <v>0.1406053285037152</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3046107791021697</v>
+        <v>0.298281665178119</v>
       </c>
       <c r="G4" t="n">
         <v>0.1235091914340451</v>
@@ -2949,7 +2949,7 @@
         <v>0.1103712366305038</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2399604590052487</v>
+        <v>0.2542916691963315</v>
       </c>
       <c r="G7" t="n">
         <v>0.7301566224057848</v>
@@ -2980,7 +2980,7 @@
         <v>0.1568990805389059</v>
       </c>
       <c r="F8" t="n">
-        <v>0.327882596873648</v>
+        <v>0.3374064063974575</v>
       </c>
       <c r="G8" t="n">
         <v>0.842779073338177</v>
@@ -3011,7 +3011,7 @@
         <v>0.1551375132818893</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3020429508982123</v>
+        <v>0.3212737201289815</v>
       </c>
       <c r="G9" t="n">
         <v>0.6489182458047602</v>
@@ -3042,7 +3042,7 @@
         <v>0.08417659076403987</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2819721384249597</v>
+        <v>0.2955590949466989</v>
       </c>
       <c r="G10" t="n">
         <v>0.8960831210606059</v>
@@ -3073,7 +3073,7 @@
         <v>0.1323595477880339</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3066354842744071</v>
+        <v>0.2931946240593533</v>
       </c>
       <c r="G11" t="n">
         <v>0.9105266699298646</v>
@@ -3104,7 +3104,7 @@
         <v>0.09528338574839093</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2554631273729394</v>
+        <v>0.28781606854941</v>
       </c>
       <c r="G12" t="n">
         <v>0.6802301810815002</v>
@@ -3135,7 +3135,7 @@
         <v>0.09175487238184334</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2703809809809795</v>
+        <v>0.2733221574515677</v>
       </c>
       <c r="G13" t="n">
         <v>0.6679287428194797</v>
@@ -3166,7 +3166,7 @@
         <v>0.08676156056606386</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2954753853313141</v>
+        <v>0.2865468139027426</v>
       </c>
       <c r="G14" t="n">
         <v>0.7093355249669493</v>
@@ -3197,7 +3197,7 @@
         <v>0.08000260405525979</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2538397078345891</v>
+        <v>0.2426037527784093</v>
       </c>
       <c r="G15" t="n">
         <v>0.9040031457786135</v>
@@ -3228,7 +3228,7 @@
         <v>0.08465585553067155</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2842114739936654</v>
+        <v>0.2931400454222368</v>
       </c>
       <c r="G16" t="n">
         <v>0.8916641153193877</v>
@@ -3259,7 +3259,7 @@
         <v>0.1407452350768398</v>
       </c>
       <c r="F17" t="n">
-        <v>0.2790852139902757</v>
+        <v>0.2878061442228339</v>
       </c>
       <c r="G17" t="n">
         <v>0.897492258943114</v>
@@ -3321,7 +3321,7 @@
         <v>0.1387763462793593</v>
       </c>
       <c r="F19" t="n">
-        <v>0.3405103737553893</v>
+        <v>0.3143198975649131</v>
       </c>
       <c r="G19" t="n">
         <v>0.6853683780231075</v>
@@ -3533,7 +3533,7 @@
         <v>0.08271242113905845</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2912176573155931</v>
+        <v>0.2904286895658676</v>
       </c>
       <c r="D2" t="n">
         <v>0.7454769729799278</v>
@@ -3542,7 +3542,7 @@
         <v>0.01600528381261872</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03683912979926751</v>
+        <v>0.03453674817974294</v>
       </c>
       <c r="G2" t="n">
         <v>0.1472831242530836</v>
@@ -3551,7 +3551,7 @@
         <v>0.05489363236837091</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2102139731320689</v>
+        <v>0.2211114090295048</v>
       </c>
       <c r="J2" t="n">
         <v>0.382831176269638</v>
@@ -3560,7 +3560,7 @@
         <v>0.1140777195744919</v>
       </c>
       <c r="L2" t="n">
-        <v>0.334253345204327</v>
+        <v>0.3421459761386313</v>
       </c>
       <c r="M2" t="n">
         <v>0.9111813439813872</v>
@@ -3626,7 +3626,7 @@
         <v>0.106606049056115</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2706720718100053</v>
+        <v>0.2821023196853642</v>
       </c>
       <c r="D3" t="n">
         <v>0.7987747512607255</v>
@@ -3635,7 +3635,7 @@
         <v>0.03244337841282056</v>
       </c>
       <c r="F3" t="n">
-        <v>0.04759407343931685</v>
+        <v>0.04434134473086152</v>
       </c>
       <c r="G3" t="n">
         <v>0.1134130249586964</v>
@@ -3644,7 +3644,7 @@
         <v>0.03821712062510718</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1684768357109067</v>
+        <v>0.1811463416957392</v>
       </c>
       <c r="J3" t="n">
         <v>0.6225818585643652</v>
@@ -3653,7 +3653,7 @@
         <v>0.1658425703011601</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3714292355243237</v>
+        <v>0.3309530450481332</v>
       </c>
       <c r="M3" t="n">
         <v>0.9081081587271729</v>
@@ -3731,7 +3731,7 @@
         <v>0.1412223822674533</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2992053002697077</v>
+        <v>0.3017864309951214</v>
       </c>
       <c r="D4" t="n">
         <v>0.7430039148056385</v>
@@ -3740,7 +3740,7 @@
         <v>0.05037100079749553</v>
       </c>
       <c r="F4" t="n">
-        <v>0.05440987523529585</v>
+        <v>0.05085246853242501</v>
       </c>
       <c r="G4" t="n">
         <v>0.1193927624697835</v>
@@ -3749,7 +3749,7 @@
         <v>0.04500653599041117</v>
       </c>
       <c r="I4" t="n">
-        <v>0.184050339770828</v>
+        <v>0.1853323910528792</v>
       </c>
       <c r="J4" t="n">
         <v>0.5760314784493452</v>
@@ -3758,7 +3758,7 @@
         <v>0.2551855286176491</v>
       </c>
       <c r="L4" t="n">
-        <v>0.4163599528234442</v>
+        <v>0.4044551909186823</v>
       </c>
       <c r="M4" t="n">
         <v>0.9083710383433946</v>
@@ -3836,7 +3836,7 @@
         <v>0.1087363205987952</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2756456905996817</v>
+        <v>0.2790080264166018</v>
       </c>
       <c r="D5" t="n">
         <v>0.7376864768980288</v>
@@ -3845,7 +3845,7 @@
         <v>0.03853663162482749</v>
       </c>
       <c r="F5" t="n">
-        <v>0.04534271882481353</v>
+        <v>0.04248480552246491</v>
       </c>
       <c r="G5" t="n">
         <v>0.1987787260761697</v>
@@ -3854,7 +3854,7 @@
         <v>0.0282416407933045</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1616512842689058</v>
+        <v>0.1680615406791622</v>
       </c>
       <c r="J5" t="n">
         <v>0.1235091914340451</v>
@@ -3863,7 +3863,7 @@
         <v>0.1689174524059005</v>
       </c>
       <c r="L5" t="n">
-        <v>0.3405103737553893</v>
+        <v>0.3374064063974575</v>
       </c>
       <c r="M5" t="n">
         <v>0.9635762266826113</v>
@@ -3974,7 +3974,7 @@
         <v>0.08271242113905845</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2912176573155931</v>
+        <v>0.2904286895658676</v>
       </c>
       <c r="D2" t="n">
         <v>0.7454769729799278</v>
@@ -3990,7 +3990,7 @@
         <v>0.106606049056115</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2706720718100053</v>
+        <v>0.2821023196853642</v>
       </c>
       <c r="D3" t="n">
         <v>0.7987747512607255</v>
@@ -4006,7 +4006,7 @@
         <v>0.1412223822674533</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2992053002697077</v>
+        <v>0.3017864309951214</v>
       </c>
       <c r="D4" t="n">
         <v>0.7430039148056385</v>
@@ -4022,7 +4022,7 @@
         <v>0.1087363205987952</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2756456905996817</v>
+        <v>0.2790080264166018</v>
       </c>
       <c r="D5" t="n">
         <v>0.7376864768980288</v>
@@ -4079,7 +4079,7 @@
         <v>0.01600528381261872</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03683912979926751</v>
+        <v>0.03453674817974294</v>
       </c>
       <c r="D2" t="n">
         <v>0.1472831242530836</v>
@@ -4095,7 +4095,7 @@
         <v>0.03244337841282056</v>
       </c>
       <c r="C3" t="n">
-        <v>0.04759407343931685</v>
+        <v>0.04434134473086152</v>
       </c>
       <c r="D3" t="n">
         <v>0.1134130249586964</v>
@@ -4111,7 +4111,7 @@
         <v>0.05037100079749553</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05440987523529585</v>
+        <v>0.05085246853242501</v>
       </c>
       <c r="D4" t="n">
         <v>0.1193927624697835</v>
@@ -4127,7 +4127,7 @@
         <v>0.03853663162482749</v>
       </c>
       <c r="C5" t="n">
-        <v>0.04534271882481353</v>
+        <v>0.04248480552246491</v>
       </c>
       <c r="D5" t="n">
         <v>0.1987787260761697</v>
@@ -4184,7 +4184,7 @@
         <v>0.05489363236837091</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2102139731320689</v>
+        <v>0.2211114090295048</v>
       </c>
       <c r="D2" t="n">
         <v>0.382831176269638</v>
@@ -4200,7 +4200,7 @@
         <v>0.03821712062510718</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1684768357109067</v>
+        <v>0.1811463416957392</v>
       </c>
       <c r="D3" t="n">
         <v>0.6225818585643652</v>
@@ -4216,7 +4216,7 @@
         <v>0.04500653599041117</v>
       </c>
       <c r="C4" t="n">
-        <v>0.184050339770828</v>
+        <v>0.1853323910528792</v>
       </c>
       <c r="D4" t="n">
         <v>0.5760314784493452</v>
@@ -4232,7 +4232,7 @@
         <v>0.0282416407933045</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1616512842689058</v>
+        <v>0.1680615406791622</v>
       </c>
       <c r="D5" t="n">
         <v>0.1235091914340451</v>
@@ -4289,7 +4289,7 @@
         <v>0.1140777195744919</v>
       </c>
       <c r="C2" t="n">
-        <v>0.334253345204327</v>
+        <v>0.3421459761386313</v>
       </c>
       <c r="D2" t="n">
         <v>0.9111813439813872</v>
@@ -4305,7 +4305,7 @@
         <v>0.1658425703011601</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3714292355243237</v>
+        <v>0.3309530450481332</v>
       </c>
       <c r="D3" t="n">
         <v>0.9081081587271729</v>
@@ -4321,7 +4321,7 @@
         <v>0.2551855286176491</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4163599528234442</v>
+        <v>0.4044551909186823</v>
       </c>
       <c r="D4" t="n">
         <v>0.9083710383433946</v>
@@ -4337,7 +4337,7 @@
         <v>0.1689174524059005</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3405103737553893</v>
+        <v>0.3374064063974575</v>
       </c>
       <c r="D5" t="n">
         <v>0.9635762266826113</v>

</xml_diff>